<commit_message>
Raspberry Pi is slower than I had thought. Make it easier.
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/Tsinghua/大三秋季学期/计算机网络原理/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/Router-Lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466D6170-C1B8-9F42-9282-5CC5647D1E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4A3424-96DB-6942-87D9-CF2687F7D2EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18740" xr2:uid="{7E4902F0-0072-F54B-B0FB-9508F23376F4}"/>
   </bookViews>
@@ -437,10 +437,10 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -562,7 +562,7 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -589,7 +589,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="1">
-        <f>3*MIN(5,F2+H2+J2+L2+N2+P2+R2)+D2*10+E2*10+10*EXP(-G2/100)+30*(1-EXP(-I2/20))+30*(1-EXP(-K2/10))+10*M2+15*O2+15*Q2+S2</f>
+        <f>3*MIN(5,F2+H2+J2+L2+N2+P2+R2)+D2*10+E2*10+10*EXP(-G2/100)+30*(1-EXP(-I2/20))+30*(1-EXP(-K2))+10*M2+15*O2+15*Q2+S2</f>
         <v>100.52261916209029</v>
       </c>
       <c r="U2" s="1">

</xml_diff>